<commit_message>
Fixed table header issue
</commit_message>
<xml_diff>
--- a/research-table/public/mapped_studies.xlsx
+++ b/research-table/public/mapped_studies.xlsx
@@ -2357,13 +2357,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BS110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A101" sqref="A101"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="6" max="6" width="44.6640625" customWidth="1"/>
+    <col min="13" max="13" width="155.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:71" x14ac:dyDescent="0.3">
@@ -2621,6 +2624,9 @@
       <c r="M2" t="s">
         <v>77</v>
       </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
       <c r="O2">
         <v>1</v>
       </c>
@@ -2680,6 +2686,9 @@
       <c r="M3" t="s">
         <v>86</v>
       </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
       <c r="O3">
         <v>1</v>
       </c>
@@ -2730,6 +2739,9 @@
       <c r="M4" t="s">
         <v>94</v>
       </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
       <c r="O4">
         <v>1</v>
       </c>
@@ -2858,6 +2870,9 @@
       <c r="M5" t="s">
         <v>102</v>
       </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
       <c r="O5">
         <v>1</v>
       </c>
@@ -2926,6 +2941,9 @@
       <c r="M6" t="s">
         <v>108</v>
       </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
       <c r="O6">
         <v>1</v>
       </c>
@@ -3024,6 +3042,9 @@
       <c r="M7" t="s">
         <v>115</v>
       </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
       <c r="O7">
         <v>1</v>
       </c>
@@ -3083,6 +3104,9 @@
       <c r="M8" t="s">
         <v>121</v>
       </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
       <c r="O8">
         <v>1</v>
       </c>
@@ -3145,6 +3169,9 @@
       <c r="M9" t="s">
         <v>128</v>
       </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
       <c r="O9">
         <v>1</v>
       </c>
@@ -3204,6 +3231,9 @@
       <c r="M10" t="s">
         <v>135</v>
       </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
       <c r="O10">
         <v>1</v>
       </c>
@@ -3260,6 +3290,9 @@
       <c r="M11" t="s">
         <v>141</v>
       </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
       <c r="O11">
         <v>1</v>
       </c>
@@ -3331,6 +3364,12 @@
       <c r="M12" t="s">
         <v>148</v>
       </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
       <c r="R12">
         <v>1</v>
       </c>
@@ -3419,6 +3458,9 @@
       <c r="M14" t="s">
         <v>159</v>
       </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
       <c r="O14">
         <v>1</v>
       </c>
@@ -3484,6 +3526,9 @@
       <c r="M15" t="s">
         <v>164</v>
       </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
       <c r="O15">
         <v>1</v>
       </c>
@@ -3534,6 +3579,9 @@
       <c r="M16" t="s">
         <v>170</v>
       </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
       <c r="O16">
         <v>1</v>
       </c>
@@ -3581,6 +3629,9 @@
       <c r="M17" t="s">
         <v>176</v>
       </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
       <c r="O17">
         <v>1</v>
       </c>
@@ -3634,6 +3685,9 @@
       <c r="M18" t="s">
         <v>182</v>
       </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
       <c r="O18">
         <v>1</v>
       </c>
@@ -3687,6 +3741,9 @@
       <c r="M19" t="s">
         <v>182</v>
       </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
       <c r="O19">
         <v>1</v>
       </c>
@@ -3740,6 +3797,9 @@
       <c r="M20" t="s">
         <v>195</v>
       </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
       <c r="O20">
         <v>1</v>
       </c>
@@ -3799,6 +3859,9 @@
       <c r="M21" t="s">
         <v>201</v>
       </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
       <c r="O21">
         <v>1</v>
       </c>
@@ -3867,6 +3930,9 @@
       <c r="M22" t="s">
         <v>208</v>
       </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
       <c r="O22">
         <v>1</v>
       </c>
@@ -3926,6 +3992,9 @@
       <c r="M23" t="s">
         <v>86</v>
       </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
       <c r="O23">
         <v>1</v>
       </c>
@@ -3952,6 +4021,9 @@
       <c r="M24" t="s">
         <v>86</v>
       </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
       <c r="O24">
         <v>1</v>
       </c>
@@ -3999,6 +4071,9 @@
       <c r="M25" t="s">
         <v>86</v>
       </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
       <c r="O25">
         <v>1</v>
       </c>
@@ -4049,6 +4124,9 @@
       <c r="M26" t="s">
         <v>86</v>
       </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
       <c r="O26">
         <v>1</v>
       </c>
@@ -4099,6 +4177,9 @@
       <c r="M27" t="s">
         <v>86</v>
       </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
       <c r="O27">
         <v>1</v>
       </c>
@@ -4253,6 +4334,9 @@
       <c r="M29" t="s">
         <v>86</v>
       </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
       <c r="O29">
         <v>1</v>
       </c>
@@ -4282,6 +4366,12 @@
       <c r="H30" t="s">
         <v>244</v>
       </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
@@ -4323,6 +4413,9 @@
       <c r="M31" t="s">
         <v>86</v>
       </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
       <c r="O31">
         <v>1</v>
       </c>
@@ -4370,6 +4463,9 @@
       <c r="M32" t="s">
         <v>86</v>
       </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
       <c r="O32">
         <v>1</v>
       </c>
@@ -4420,6 +4516,9 @@
       <c r="M33" t="s">
         <v>86</v>
       </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
       <c r="O33">
         <v>1</v>
       </c>
@@ -4470,6 +4569,9 @@
       <c r="M34" t="s">
         <v>86</v>
       </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
       <c r="O34">
         <v>1</v>
       </c>
@@ -4520,6 +4622,9 @@
       <c r="M35" t="s">
         <v>182</v>
       </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
       <c r="O35">
         <v>1</v>
       </c>
@@ -4558,6 +4663,9 @@
       <c r="M36" t="s">
         <v>86</v>
       </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
       <c r="O36">
         <v>1</v>
       </c>
@@ -4729,6 +4837,9 @@
       <c r="M39" t="s">
         <v>293</v>
       </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
       <c r="O39">
         <v>1</v>
       </c>
@@ -4797,6 +4908,9 @@
       <c r="M40" t="s">
         <v>300</v>
       </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
       <c r="O40">
         <v>1</v>
       </c>
@@ -4906,6 +5020,9 @@
       <c r="M42" t="s">
         <v>311</v>
       </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
       <c r="O42">
         <v>1</v>
       </c>
@@ -5192,6 +5309,9 @@
       <c r="M44" t="s">
         <v>321</v>
       </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
       <c r="O44">
         <v>1</v>
       </c>
@@ -5337,6 +5457,9 @@
       <c r="M46" t="s">
         <v>331</v>
       </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
       <c r="O46">
         <v>1</v>
       </c>
@@ -5547,6 +5670,9 @@
       <c r="M49" t="s">
         <v>350</v>
       </c>
+      <c r="N49">
+        <v>0</v>
+      </c>
       <c r="O49">
         <v>1</v>
       </c>
@@ -5716,6 +5842,12 @@
       <c r="M51" t="s">
         <v>362</v>
       </c>
+      <c r="N51">
+        <v>0</v>
+      </c>
+      <c r="O51">
+        <v>0</v>
+      </c>
       <c r="U51">
         <v>1</v>
       </c>
@@ -5745,6 +5877,12 @@
       <c r="H52" t="s">
         <v>361</v>
       </c>
+      <c r="N52">
+        <v>0</v>
+      </c>
+      <c r="O52">
+        <v>0</v>
+      </c>
     </row>
     <row r="53" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
@@ -5938,6 +6076,9 @@
       <c r="M54" t="s">
         <v>86</v>
       </c>
+      <c r="N54">
+        <v>0</v>
+      </c>
       <c r="O54">
         <v>1</v>
       </c>
@@ -5970,6 +6111,9 @@
       <c r="M55" t="s">
         <v>380</v>
       </c>
+      <c r="N55">
+        <v>0</v>
+      </c>
       <c r="O55">
         <v>1</v>
       </c>
@@ -6068,6 +6212,9 @@
       <c r="M56" t="s">
         <v>385</v>
       </c>
+      <c r="N56">
+        <v>0</v>
+      </c>
       <c r="O56">
         <v>1</v>
       </c>
@@ -6163,6 +6310,9 @@
       <c r="M57" t="s">
         <v>391</v>
       </c>
+      <c r="N57">
+        <v>0</v>
+      </c>
       <c r="O57">
         <v>1</v>
       </c>
@@ -6216,6 +6366,9 @@
       <c r="M58" t="s">
         <v>396</v>
       </c>
+      <c r="N58">
+        <v>0</v>
+      </c>
       <c r="O58">
         <v>1</v>
       </c>
@@ -6314,6 +6467,9 @@
       <c r="M59" t="s">
         <v>401</v>
       </c>
+      <c r="N59">
+        <v>0</v>
+      </c>
       <c r="O59">
         <v>1</v>
       </c>
@@ -6418,6 +6574,9 @@
       <c r="M60" t="s">
         <v>406</v>
       </c>
+      <c r="N60">
+        <v>0</v>
+      </c>
       <c r="O60">
         <v>1</v>
       </c>
@@ -6525,6 +6684,9 @@
       <c r="M61" t="s">
         <v>86</v>
       </c>
+      <c r="N61">
+        <v>0</v>
+      </c>
       <c r="O61">
         <v>1</v>
       </c>
@@ -6557,6 +6719,9 @@
       <c r="M62" t="s">
         <v>416</v>
       </c>
+      <c r="N62">
+        <v>0</v>
+      </c>
       <c r="O62">
         <v>1</v>
       </c>
@@ -6658,6 +6823,9 @@
       <c r="M63" t="s">
         <v>421</v>
       </c>
+      <c r="N63">
+        <v>0</v>
+      </c>
       <c r="O63">
         <v>1</v>
       </c>
@@ -6759,6 +6927,9 @@
       <c r="M64" t="s">
         <v>427</v>
       </c>
+      <c r="N64">
+        <v>0</v>
+      </c>
       <c r="O64">
         <v>1</v>
       </c>
@@ -6913,6 +7084,12 @@
       <c r="M66" t="s">
         <v>438</v>
       </c>
+      <c r="N66">
+        <v>0</v>
+      </c>
+      <c r="O66">
+        <v>0</v>
+      </c>
       <c r="R66">
         <v>1</v>
       </c>
@@ -7007,6 +7184,12 @@
       <c r="H68" t="s">
         <v>450</v>
       </c>
+      <c r="N68">
+        <v>0</v>
+      </c>
+      <c r="O68">
+        <v>0</v>
+      </c>
     </row>
     <row r="69" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
@@ -7048,6 +7231,12 @@
       <c r="M69" t="s">
         <v>306</v>
       </c>
+      <c r="N69">
+        <v>0</v>
+      </c>
+      <c r="O69">
+        <v>0</v>
+      </c>
       <c r="S69">
         <v>1</v>
       </c>
@@ -7092,6 +7281,9 @@
       <c r="M70" t="s">
         <v>462</v>
       </c>
+      <c r="N70">
+        <v>0</v>
+      </c>
       <c r="O70">
         <v>1</v>
       </c>
@@ -7199,6 +7391,9 @@
       <c r="M71" t="s">
         <v>86</v>
       </c>
+      <c r="N71">
+        <v>0</v>
+      </c>
       <c r="O71">
         <v>1</v>
       </c>
@@ -7231,6 +7426,9 @@
       <c r="M72" t="s">
         <v>86</v>
       </c>
+      <c r="N72">
+        <v>0</v>
+      </c>
       <c r="O72">
         <v>1</v>
       </c>
@@ -7278,6 +7476,9 @@
       <c r="M73" t="s">
         <v>86</v>
       </c>
+      <c r="N73">
+        <v>0</v>
+      </c>
       <c r="O73">
         <v>1</v>
       </c>
@@ -7310,6 +7511,9 @@
       <c r="M74" t="s">
         <v>481</v>
       </c>
+      <c r="N74">
+        <v>0</v>
+      </c>
       <c r="O74">
         <v>1</v>
       </c>
@@ -7384,6 +7588,9 @@
       <c r="M75" t="s">
         <v>487</v>
       </c>
+      <c r="N75">
+        <v>0</v>
+      </c>
       <c r="O75">
         <v>1</v>
       </c>
@@ -7461,6 +7668,9 @@
       <c r="M76" t="s">
         <v>86</v>
       </c>
+      <c r="N76">
+        <v>0</v>
+      </c>
       <c r="O76">
         <v>1</v>
       </c>
@@ -7511,6 +7721,9 @@
       <c r="M77" t="s">
         <v>499</v>
       </c>
+      <c r="N77">
+        <v>0</v>
+      </c>
       <c r="O77">
         <v>1</v>
       </c>
@@ -7561,6 +7774,9 @@
       <c r="M78" t="s">
         <v>182</v>
       </c>
+      <c r="N78">
+        <v>0</v>
+      </c>
       <c r="O78">
         <v>1</v>
       </c>
@@ -7611,6 +7827,9 @@
       <c r="M79" t="s">
         <v>182</v>
       </c>
+      <c r="N79">
+        <v>0</v>
+      </c>
       <c r="O79">
         <v>1</v>
       </c>
@@ -7646,6 +7865,9 @@
       <c r="M80" t="s">
         <v>176</v>
       </c>
+      <c r="N80">
+        <v>0</v>
+      </c>
       <c r="O80">
         <v>1</v>
       </c>
@@ -7875,6 +8097,9 @@
       <c r="M82" t="s">
         <v>86</v>
       </c>
+      <c r="N82">
+        <v>0</v>
+      </c>
       <c r="O82">
         <v>1</v>
       </c>
@@ -7904,6 +8129,9 @@
       <c r="M83" t="s">
         <v>86</v>
       </c>
+      <c r="N83">
+        <v>0</v>
+      </c>
       <c r="O83">
         <v>1</v>
       </c>
@@ -7954,6 +8182,9 @@
       <c r="M84" t="s">
         <v>534</v>
       </c>
+      <c r="N84">
+        <v>0</v>
+      </c>
       <c r="O84">
         <v>1</v>
       </c>
@@ -8010,6 +8241,9 @@
       <c r="M85" t="s">
         <v>170</v>
       </c>
+      <c r="N85">
+        <v>0</v>
+      </c>
       <c r="O85">
         <v>1</v>
       </c>
@@ -8092,6 +8326,9 @@
       <c r="M87" t="s">
         <v>548</v>
       </c>
+      <c r="N87">
+        <v>0</v>
+      </c>
       <c r="O87">
         <v>1</v>
       </c>
@@ -8169,6 +8406,9 @@
       <c r="M88" t="s">
         <v>552</v>
       </c>
+      <c r="N88">
+        <v>0</v>
+      </c>
       <c r="O88">
         <v>1</v>
       </c>
@@ -8346,6 +8586,9 @@
       <c r="M91" t="s">
         <v>566</v>
       </c>
+      <c r="N91">
+        <v>0</v>
+      </c>
       <c r="O91">
         <v>1</v>
       </c>
@@ -8390,6 +8633,12 @@
       <c r="M92" t="s">
         <v>572</v>
       </c>
+      <c r="N92">
+        <v>0</v>
+      </c>
+      <c r="O92">
+        <v>0</v>
+      </c>
       <c r="R92">
         <v>1</v>
       </c>
@@ -8455,6 +8704,9 @@
       <c r="M93" t="s">
         <v>577</v>
       </c>
+      <c r="N93">
+        <v>0</v>
+      </c>
       <c r="O93">
         <v>1</v>
       </c>
@@ -8602,6 +8854,9 @@
       <c r="M96" t="s">
         <v>591</v>
       </c>
+      <c r="N96">
+        <v>0</v>
+      </c>
       <c r="O96">
         <v>1</v>
       </c>
@@ -8667,6 +8922,9 @@
       <c r="N97">
         <v>1</v>
       </c>
+      <c r="O97">
+        <v>0</v>
+      </c>
       <c r="S97">
         <v>1</v>
       </c>
@@ -8696,6 +8954,9 @@
       <c r="M98" t="s">
         <v>601</v>
       </c>
+      <c r="N98">
+        <v>0</v>
+      </c>
       <c r="O98">
         <v>1</v>
       </c>
@@ -8779,6 +9040,9 @@
       <c r="M99" t="s">
         <v>86</v>
       </c>
+      <c r="N99">
+        <v>0</v>
+      </c>
       <c r="O99">
         <v>1</v>
       </c>
@@ -8949,6 +9213,9 @@
       <c r="M103" t="s">
         <v>624</v>
       </c>
+      <c r="N103">
+        <v>0</v>
+      </c>
       <c r="O103">
         <v>1</v>
       </c>
@@ -9096,6 +9363,9 @@
       <c r="M106" t="s">
         <v>639</v>
       </c>
+      <c r="N106">
+        <v>0</v>
+      </c>
       <c r="O106">
         <v>1</v>
       </c>
@@ -9149,6 +9419,9 @@
       <c r="M107" t="s">
         <v>643</v>
       </c>
+      <c r="N107">
+        <v>0</v>
+      </c>
       <c r="O107">
         <v>1</v>
       </c>
@@ -9205,6 +9478,9 @@
       <c r="M108" t="s">
         <v>647</v>
       </c>
+      <c r="N108">
+        <v>0</v>
+      </c>
       <c r="O108">
         <v>1</v>
       </c>
@@ -9344,5 +9620,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated ocean studies and latest study
</commit_message>
<xml_diff>
--- a/research-table/public/mapped_studies.xlsx
+++ b/research-table/public/mapped_studies.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BS110"/>
+  <dimension ref="A1:BT110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -787,6 +787,11 @@
       <c r="BS1" s="1" t="inlineStr">
         <is>
           <t>Lithium (Li)</t>
+        </is>
+      </c>
+      <c r="BT1" s="1" t="inlineStr">
+        <is>
+          <t>Boron (B)</t>
         </is>
       </c>
     </row>
@@ -918,6 +923,7 @@
       <c r="BQ2" t="inlineStr"/>
       <c r="BR2" t="inlineStr"/>
       <c r="BS2" t="inlineStr"/>
+      <c r="BT2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1041,6 +1047,7 @@
       <c r="BQ3" t="inlineStr"/>
       <c r="BR3" t="inlineStr"/>
       <c r="BS3" t="inlineStr"/>
+      <c r="BT3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1216,6 +1223,7 @@
       <c r="BQ4" t="inlineStr"/>
       <c r="BR4" t="inlineStr"/>
       <c r="BS4" t="inlineStr"/>
+      <c r="BT4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1351,6 +1359,7 @@
       <c r="BQ5" t="inlineStr"/>
       <c r="BR5" t="inlineStr"/>
       <c r="BS5" t="inlineStr"/>
+      <c r="BT5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1506,6 +1515,7 @@
       <c r="BQ6" t="inlineStr"/>
       <c r="BR6" t="inlineStr"/>
       <c r="BS6" t="inlineStr"/>
+      <c r="BT6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1635,6 +1645,7 @@
       <c r="BQ7" t="inlineStr"/>
       <c r="BR7" t="inlineStr"/>
       <c r="BS7" t="inlineStr"/>
+      <c r="BT7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1766,6 +1777,7 @@
       <c r="BQ8" t="inlineStr"/>
       <c r="BR8" t="inlineStr"/>
       <c r="BS8" t="inlineStr"/>
+      <c r="BT8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1895,6 +1907,7 @@
       <c r="BQ9" t="inlineStr"/>
       <c r="BR9" t="inlineStr"/>
       <c r="BS9" t="inlineStr"/>
+      <c r="BT9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1922,7 +1935,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> North Atlantic| South Atlantic| Medeterranian, Black and Caspian Sea|</t>
+          <t xml:space="preserve"> North Atlantic| South Atlantic| Mediterranean and Others|</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -2022,6 +2035,7 @@
       <c r="BQ10" t="inlineStr"/>
       <c r="BR10" t="inlineStr"/>
       <c r="BS10" t="inlineStr"/>
+      <c r="BT10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2159,6 +2173,7 @@
       <c r="BQ11" t="inlineStr"/>
       <c r="BR11" t="inlineStr"/>
       <c r="BS11" t="inlineStr"/>
+      <c r="BT11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2274,6 +2289,7 @@
       <c r="BQ12" t="inlineStr"/>
       <c r="BR12" t="inlineStr"/>
       <c r="BS12" t="inlineStr"/>
+      <c r="BT12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2391,6 +2407,7 @@
       <c r="BQ13" t="inlineStr"/>
       <c r="BR13" t="inlineStr"/>
       <c r="BS13" t="inlineStr"/>
+      <c r="BT13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2526,6 +2543,7 @@
       <c r="BQ14" t="inlineStr"/>
       <c r="BR14" t="inlineStr"/>
       <c r="BS14" t="inlineStr"/>
+      <c r="BT14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2549,7 +2567,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Medeterranian, Black and Caspian Sea|</t>
+          <t xml:space="preserve"> Mediterranean and Others|</t>
         </is>
       </c>
       <c r="G15" t="n">
@@ -2641,6 +2659,7 @@
       <c r="BQ15" t="inlineStr"/>
       <c r="BR15" t="inlineStr"/>
       <c r="BS15" t="inlineStr"/>
+      <c r="BT15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2760,6 +2779,7 @@
       <c r="BQ16" t="inlineStr"/>
       <c r="BR16" t="inlineStr"/>
       <c r="BS16" t="inlineStr"/>
+      <c r="BT16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2879,6 +2899,7 @@
       <c r="BQ17" t="inlineStr"/>
       <c r="BR17" t="inlineStr"/>
       <c r="BS17" t="inlineStr"/>
+      <c r="BT17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -3004,6 +3025,7 @@
       <c r="BQ18" t="inlineStr"/>
       <c r="BR18" t="inlineStr"/>
       <c r="BS18" t="inlineStr"/>
+      <c r="BT18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -3129,6 +3151,7 @@
       <c r="BQ19" t="inlineStr"/>
       <c r="BR19" t="inlineStr"/>
       <c r="BS19" t="inlineStr"/>
+      <c r="BT19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -3258,6 +3281,7 @@
       <c r="BQ20" t="inlineStr"/>
       <c r="BR20" t="inlineStr"/>
       <c r="BS20" t="inlineStr"/>
+      <c r="BT20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -3393,6 +3417,7 @@
       <c r="BQ21" t="inlineStr"/>
       <c r="BR21" t="inlineStr"/>
       <c r="BS21" t="inlineStr"/>
+      <c r="BT21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3532,6 +3557,7 @@
       <c r="BQ22" t="inlineStr"/>
       <c r="BR22" t="inlineStr"/>
       <c r="BS22" t="inlineStr"/>
+      <c r="BT22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3639,6 +3665,7 @@
       <c r="BQ23" t="inlineStr"/>
       <c r="BR23" t="inlineStr"/>
       <c r="BS23" t="inlineStr"/>
+      <c r="BT23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3738,6 +3765,7 @@
       <c r="BQ24" t="inlineStr"/>
       <c r="BR24" t="inlineStr"/>
       <c r="BS24" t="inlineStr"/>
+      <c r="BT24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3861,6 +3889,7 @@
       <c r="BQ25" t="inlineStr"/>
       <c r="BR25" t="inlineStr"/>
       <c r="BS25" t="inlineStr"/>
+      <c r="BT25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3984,6 +4013,7 @@
       <c r="BQ26" t="inlineStr"/>
       <c r="BR26" t="inlineStr"/>
       <c r="BS26" t="inlineStr"/>
+      <c r="BT26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -4103,6 +4133,7 @@
       <c r="BQ27" t="inlineStr"/>
       <c r="BR27" t="inlineStr"/>
       <c r="BS27" t="inlineStr"/>
+      <c r="BT27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -4262,6 +4293,7 @@
       <c r="BQ28" t="inlineStr"/>
       <c r="BR28" t="inlineStr"/>
       <c r="BS28" t="inlineStr"/>
+      <c r="BT28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -4381,6 +4413,7 @@
       <c r="BQ29" t="inlineStr"/>
       <c r="BR29" t="inlineStr"/>
       <c r="BS29" t="inlineStr"/>
+      <c r="BT29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -4478,6 +4511,7 @@
       <c r="BQ30" t="inlineStr"/>
       <c r="BR30" t="inlineStr"/>
       <c r="BS30" t="inlineStr"/>
+      <c r="BT30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -4597,6 +4631,7 @@
       <c r="BQ31" t="inlineStr"/>
       <c r="BR31" t="inlineStr"/>
       <c r="BS31" t="inlineStr"/>
+      <c r="BT31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -4720,6 +4755,7 @@
       <c r="BQ32" t="inlineStr"/>
       <c r="BR32" t="inlineStr"/>
       <c r="BS32" t="inlineStr"/>
+      <c r="BT32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -4843,6 +4879,7 @@
       <c r="BQ33" t="inlineStr"/>
       <c r="BR33" t="inlineStr"/>
       <c r="BS33" t="inlineStr"/>
+      <c r="BT33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -4870,7 +4907,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Medeterranian, Black and Caspian Sea|</t>
+          <t xml:space="preserve"> Mediterranean and Others|</t>
         </is>
       </c>
       <c r="G34" t="n">
@@ -4966,6 +5003,7 @@
       <c r="BQ34" t="inlineStr"/>
       <c r="BR34" t="inlineStr"/>
       <c r="BS34" t="inlineStr"/>
+      <c r="BT34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4993,7 +5031,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Medeterranian, Black and Caspian Sea|</t>
+          <t xml:space="preserve"> Mediterranean and Others|</t>
         </is>
       </c>
       <c r="G35" t="n">
@@ -5091,6 +5129,7 @@
       <c r="BQ35" t="inlineStr"/>
       <c r="BR35" t="inlineStr"/>
       <c r="BS35" t="inlineStr"/>
+      <c r="BT35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -5202,6 +5241,7 @@
       <c r="BQ36" t="inlineStr"/>
       <c r="BR36" t="inlineStr"/>
       <c r="BS36" t="inlineStr"/>
+      <c r="BT36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -5345,6 +5385,7 @@
       <c r="BQ37" t="inlineStr"/>
       <c r="BR37" t="inlineStr"/>
       <c r="BS37" t="inlineStr"/>
+      <c r="BT37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -5470,6 +5511,7 @@
       <c r="BQ38" t="inlineStr"/>
       <c r="BR38" t="inlineStr"/>
       <c r="BS38" t="inlineStr"/>
+      <c r="BT38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -5591,6 +5633,7 @@
       <c r="BQ39" t="inlineStr"/>
       <c r="BR39" t="inlineStr"/>
       <c r="BS39" t="inlineStr"/>
+      <c r="BT39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -5732,6 +5775,7 @@
       <c r="BQ40" t="inlineStr"/>
       <c r="BR40" t="inlineStr"/>
       <c r="BS40" t="inlineStr"/>
+      <c r="BT40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -5849,6 +5893,7 @@
       <c r="BQ41" t="inlineStr"/>
       <c r="BR41" t="inlineStr"/>
       <c r="BS41" t="inlineStr"/>
+      <c r="BT41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -5889,7 +5934,7 @@
       <c r="L42" t="inlineStr"/>
       <c r="M42" t="inlineStr">
         <is>
-          <t>Na,  Mg,  A1,  K,  Ca,  Sc, Ti,  V,  Cr,  Mn, Fe,  Ni,  Cu,  Zn,  Ge,  As,  Se,  Mo,  Ru,  Cd,  Sn,  Sb,  Cs,  Ba,  La,  Ce, Sm,  Eu,  Hf,  Pb,  and Th</t>
+          <t>Na,  Mg,  A1,  K,  Ca,  Sc, Ti,  V,  Cr,  Mn, Fe,  Ni,  Cu,  Zn,  Ge,  As,  Se,  Mo,  Ru,  Cd,  Sn,  Sb,  Cs,  Ba,  La,  Ce, Sm,  Eu,  Hf,  Pb,  Th</t>
         </is>
       </c>
       <c r="N42" t="inlineStr"/>
@@ -6020,6 +6065,7 @@
       <c r="BQ42" t="inlineStr"/>
       <c r="BR42" t="inlineStr"/>
       <c r="BS42" t="inlineStr"/>
+      <c r="BT42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -6207,6 +6253,7 @@
       <c r="BQ43" t="inlineStr"/>
       <c r="BR43" t="inlineStr"/>
       <c r="BS43" t="inlineStr"/>
+      <c r="BT43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -6234,7 +6281,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Medeterranian, Black and Caspian Sea|</t>
+          <t xml:space="preserve"> Mediterranean and Others|</t>
         </is>
       </c>
       <c r="G44" t="n">
@@ -6338,6 +6385,7 @@
       <c r="BQ44" t="inlineStr"/>
       <c r="BR44" t="inlineStr"/>
       <c r="BS44" t="inlineStr"/>
+      <c r="BT44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -6365,7 +6413,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Medeterranian, Black and Caspian Sea|</t>
+          <t xml:space="preserve"> Mediterranean and Others|</t>
         </is>
       </c>
       <c r="G45" t="n">
@@ -6479,6 +6527,7 @@
       <c r="BQ45" t="inlineStr"/>
       <c r="BR45" t="inlineStr"/>
       <c r="BS45" t="inlineStr"/>
+      <c r="BT45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -6506,7 +6555,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Medeterranian, Black and Caspian Sea|</t>
+          <t xml:space="preserve"> Mediterranean and Others|</t>
         </is>
       </c>
       <c r="G46" t="n">
@@ -6622,6 +6671,7 @@
       <c r="BQ46" t="inlineStr"/>
       <c r="BR46" t="inlineStr"/>
       <c r="BS46" t="inlineStr"/>
+      <c r="BT46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -6759,6 +6809,7 @@
       <c r="BQ47" t="inlineStr"/>
       <c r="BR47" t="inlineStr"/>
       <c r="BS47" t="inlineStr"/>
+      <c r="BT47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -6786,7 +6837,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> North Atlantic| Medeterranian, Black and Caspian Sea|</t>
+          <t xml:space="preserve"> North Atlantic| Mediterranean and Others|</t>
         </is>
       </c>
       <c r="G48" t="n">
@@ -6886,6 +6937,7 @@
       <c r="BQ48" t="inlineStr"/>
       <c r="BR48" t="inlineStr"/>
       <c r="BS48" t="inlineStr"/>
+      <c r="BT48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -6913,7 +6965,7 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> North Atlantic| South Atlantic|</t>
+          <t xml:space="preserve"> North Atlantic| South Atlantic| Mediterranean and Others|</t>
         </is>
       </c>
       <c r="G49" t="n">
@@ -7021,6 +7073,7 @@
       <c r="BQ49" t="inlineStr"/>
       <c r="BR49" t="inlineStr"/>
       <c r="BS49" t="inlineStr"/>
+      <c r="BT49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -7046,7 +7099,11 @@
           <t>https://analyticalsciencejournals.onlinelibrary.wiley.com/doi/abs/10.1002/(SICI)1097-4539(199807/08)27:4%3C236::AID-XRS292%3E3.0.CO;2-F</t>
         </is>
       </c>
-      <c r="F50" t="inlineStr"/>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Mediterranean and Others|</t>
+        </is>
+      </c>
       <c r="G50" t="n">
         <v>0</v>
       </c>
@@ -7182,6 +7239,7 @@
       <c r="BQ50" t="inlineStr"/>
       <c r="BR50" t="inlineStr"/>
       <c r="BS50" t="inlineStr"/>
+      <c r="BT50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -7289,6 +7347,7 @@
       <c r="BQ51" t="inlineStr"/>
       <c r="BR51" t="inlineStr"/>
       <c r="BS51" t="inlineStr"/>
+      <c r="BT51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -7384,6 +7443,7 @@
       <c r="BQ52" t="inlineStr"/>
       <c r="BR52" t="inlineStr"/>
       <c r="BS52" t="inlineStr"/>
+      <c r="BT52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -7581,6 +7641,7 @@
       <c r="BQ53" t="inlineStr"/>
       <c r="BR53" t="inlineStr"/>
       <c r="BS53" t="inlineStr"/>
+      <c r="BT53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -7688,6 +7749,7 @@
       <c r="BQ54" t="inlineStr"/>
       <c r="BR54" t="inlineStr"/>
       <c r="BS54" t="inlineStr"/>
+      <c r="BT54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -7839,6 +7901,7 @@
       <c r="BQ55" t="inlineStr"/>
       <c r="BR55" t="inlineStr"/>
       <c r="BS55" t="inlineStr"/>
+      <c r="BT55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -7980,6 +8043,7 @@
       <c r="BQ56" t="inlineStr"/>
       <c r="BR56" t="inlineStr"/>
       <c r="BS56" t="inlineStr"/>
+      <c r="BT56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -8005,7 +8069,11 @@
           <t>https://www.sciencedirect.com/science/article/abs/pii/S0168583X97002541</t>
         </is>
       </c>
-      <c r="F57" t="inlineStr"/>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Mediterranean and Others|</t>
+        </is>
+      </c>
       <c r="G57" t="n">
         <v>1</v>
       </c>
@@ -8109,6 +8177,7 @@
       <c r="BQ57" t="inlineStr"/>
       <c r="BR57" t="inlineStr"/>
       <c r="BS57" t="inlineStr"/>
+      <c r="BT57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -8260,6 +8329,7 @@
       <c r="BQ58" t="inlineStr"/>
       <c r="BR58" t="inlineStr"/>
       <c r="BS58" t="inlineStr"/>
+      <c r="BT58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -8415,6 +8485,7 @@
       <c r="BQ59" t="inlineStr"/>
       <c r="BR59" t="inlineStr"/>
       <c r="BS59" t="inlineStr"/>
+      <c r="BT59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -8572,6 +8643,7 @@
       <c r="BQ60" t="inlineStr"/>
       <c r="BR60" t="inlineStr"/>
       <c r="BS60" t="inlineStr"/>
+      <c r="BT60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -8679,6 +8751,7 @@
       <c r="BQ61" t="inlineStr"/>
       <c r="BR61" t="inlineStr"/>
       <c r="BS61" t="inlineStr"/>
+      <c r="BT61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -8832,6 +8905,7 @@
       <c r="BQ62" t="inlineStr"/>
       <c r="BR62" t="inlineStr"/>
       <c r="BS62" t="inlineStr"/>
+      <c r="BT62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -8975,6 +9049,7 @@
       <c r="BQ63" t="inlineStr"/>
       <c r="BR63" t="inlineStr"/>
       <c r="BS63" t="inlineStr"/>
+      <c r="BT63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -9002,7 +9077,7 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Indian Ocean|</t>
+          <t xml:space="preserve"> Central West Pacific| Indian Ocean|</t>
         </is>
       </c>
       <c r="G64" t="n">
@@ -9118,6 +9193,7 @@
       <c r="BQ64" t="inlineStr"/>
       <c r="BR64" t="inlineStr"/>
       <c r="BS64" t="inlineStr"/>
+      <c r="BT64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -9253,6 +9329,7 @@
       <c r="BQ65" t="inlineStr"/>
       <c r="BR65" t="inlineStr"/>
       <c r="BS65" t="inlineStr"/>
+      <c r="BT65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -9280,7 +9357,7 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Medeterranian, Black and Caspian Sea|</t>
+          <t xml:space="preserve"> Mediterranean and Others|</t>
         </is>
       </c>
       <c r="G66" t="n">
@@ -9370,6 +9447,7 @@
       <c r="BQ66" t="inlineStr"/>
       <c r="BR66" t="inlineStr"/>
       <c r="BS66" t="inlineStr"/>
+      <c r="BT66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -9503,6 +9581,7 @@
       <c r="BQ67" t="inlineStr"/>
       <c r="BR67" t="inlineStr"/>
       <c r="BS67" t="inlineStr"/>
+      <c r="BT67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -9600,6 +9679,7 @@
       <c r="BQ68" t="inlineStr"/>
       <c r="BR68" t="inlineStr"/>
       <c r="BS68" t="inlineStr"/>
+      <c r="BT68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -9715,6 +9795,7 @@
       <c r="BQ69" t="inlineStr"/>
       <c r="BR69" t="inlineStr"/>
       <c r="BS69" t="inlineStr"/>
+      <c r="BT69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -9874,6 +9955,9 @@
       </c>
       <c r="BR70" t="inlineStr"/>
       <c r="BS70" t="inlineStr"/>
+      <c r="BT70" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -9993,6 +10077,7 @@
       <c r="BQ71" t="inlineStr"/>
       <c r="BR71" t="inlineStr"/>
       <c r="BS71" t="inlineStr"/>
+      <c r="BT71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -10100,6 +10185,7 @@
       <c r="BQ72" t="inlineStr"/>
       <c r="BR72" t="inlineStr"/>
       <c r="BS72" t="inlineStr"/>
+      <c r="BT72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -10127,7 +10213,7 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Bay of Bengal|</t>
+          <t xml:space="preserve"> Central West Pacific|</t>
         </is>
       </c>
       <c r="G73" t="n">
@@ -10219,11 +10305,12 @@
       <c r="BQ73" t="inlineStr"/>
       <c r="BR73" t="inlineStr"/>
       <c r="BS73" t="inlineStr"/>
+      <c r="BT73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Theodosi et al. 2010</t>
+          <t>Theodosi et al. (2010)</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -10244,7 +10331,11 @@
           <t>https://www.sciencedirect.com/science/article/pii/S0304420310000216</t>
         </is>
       </c>
-      <c r="F74" t="inlineStr"/>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Mediterranean and Others|</t>
+        </is>
+      </c>
       <c r="G74" t="n">
         <v>1</v>
       </c>
@@ -10253,10 +10344,18 @@
           <t>Marine Chemistry</t>
         </is>
       </c>
-      <c r="I74" t="inlineStr"/>
-      <c r="J74" t="inlineStr"/>
-      <c r="K74" t="inlineStr"/>
-      <c r="L74" t="inlineStr"/>
+      <c r="I74" t="n">
+        <v>35.3</v>
+      </c>
+      <c r="J74" t="n">
+        <v>35.3</v>
+      </c>
+      <c r="K74" t="n">
+        <v>25.67</v>
+      </c>
+      <c r="L74" t="n">
+        <v>25.67</v>
+      </c>
       <c r="M74" t="inlineStr">
         <is>
           <t>Fe, Mn, Cu, Ni, Zn, Pb, Cr, V, Cd,</t>
@@ -10346,6 +10445,7 @@
       <c r="BQ74" t="inlineStr"/>
       <c r="BR74" t="inlineStr"/>
       <c r="BS74" t="inlineStr"/>
+      <c r="BT74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -10398,7 +10498,7 @@
       </c>
       <c r="M75" t="inlineStr">
         <is>
-          <t>Al,  Ti,  Fe,  Mn,  Co,  Ni,  Cu,  Zn,  Cd,  and Pb</t>
+          <t>Al,  Ti,  Fe,  Mn,  Co,  Ni,  Cu,  Zn,  Cd,  Pb</t>
         </is>
       </c>
       <c r="N75" t="inlineStr"/>
@@ -10487,6 +10587,7 @@
       <c r="BQ75" t="inlineStr"/>
       <c r="BR75" t="inlineStr"/>
       <c r="BS75" t="inlineStr"/>
+      <c r="BT75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -10610,6 +10711,7 @@
       <c r="BQ76" t="inlineStr"/>
       <c r="BR76" t="inlineStr"/>
       <c r="BS76" t="inlineStr"/>
+      <c r="BT76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -10637,7 +10739,7 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Medeterranian, Black and Caspian Sea|</t>
+          <t xml:space="preserve"> Mediterranean and Others|</t>
         </is>
       </c>
       <c r="G77" t="n">
@@ -10733,6 +10835,7 @@
       <c r="BQ77" t="inlineStr"/>
       <c r="BR77" t="inlineStr"/>
       <c r="BS77" t="inlineStr"/>
+      <c r="BT77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -10850,6 +10953,7 @@
       <c r="BQ78" t="inlineStr"/>
       <c r="BR78" t="inlineStr"/>
       <c r="BS78" t="inlineStr"/>
+      <c r="BT78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -10971,6 +11075,7 @@
       <c r="BQ79" t="inlineStr"/>
       <c r="BR79" t="inlineStr"/>
       <c r="BS79" t="inlineStr"/>
+      <c r="BT79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -11078,6 +11183,7 @@
       <c r="BQ80" t="inlineStr"/>
       <c r="BR80" t="inlineStr"/>
       <c r="BS80" t="inlineStr"/>
+      <c r="BT80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -11130,7 +11236,7 @@
       </c>
       <c r="M81" t="inlineStr">
         <is>
-          <t>:Na,  Mg,  A1,  Si,  P,  S,  C1, K,  Ca,  Sc,  Ti,  V,  Cr,  Mn,  Fe, Co,  Ni,  Cu,  Zn,  Ga,  As,  Se,  Br,  Rb,  Sr,  Y,  Zr,  Nb,  Mo,  Ag,  Cd, In,  Sb,  I,  Cs,  Ba,  La,  Ce,  Sm,  Eu,  Lu,  W,  Au,  Pb,  Th</t>
+          <t>Na,  Mg,  Al,  Si,  P,  S,  Cl, K,  Ca,  Sc,  Ti,  V,  Cr,  Mn,  Fe, Co,  Ni,  Cu,  Zn,  Ga,  As,  Se,  Br,  Rb,  Sr,  Y,  Zr,  Nb,  Mo,  Ag,  Cd, In,  Sb,  I,  Cs,  Ba,  La,  Ce,  Sm,  Eu,  Lu,  W,  Au,  Pb,  Th</t>
         </is>
       </c>
       <c r="N81" t="n">
@@ -11285,6 +11391,7 @@
         <v>1</v>
       </c>
       <c r="BS81" t="inlineStr"/>
+      <c r="BT81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -11312,7 +11419,7 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t xml:space="preserve"> South Pacific| North Atlantic| South Atlantic| Medeterranian, Black and Caspian Sea|</t>
+          <t xml:space="preserve"> South Pacific| North Atlantic| South Atlantic| Mediterranean and Others|</t>
         </is>
       </c>
       <c r="G82" t="n">
@@ -11408,6 +11515,7 @@
       <c r="BQ82" t="inlineStr"/>
       <c r="BR82" t="inlineStr"/>
       <c r="BS82" t="inlineStr"/>
+      <c r="BT82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -11511,6 +11619,7 @@
       <c r="BQ83" t="inlineStr"/>
       <c r="BR83" t="inlineStr"/>
       <c r="BS83" t="inlineStr"/>
+      <c r="BT83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -11538,7 +11647,7 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Australia Pacific| Indian Ocean|</t>
+          <t xml:space="preserve"> Indian Ocean|</t>
         </is>
       </c>
       <c r="G84" t="n">
@@ -11646,11 +11755,12 @@
       <c r="BQ84" t="inlineStr"/>
       <c r="BR84" t="inlineStr"/>
       <c r="BS84" t="inlineStr"/>
+      <c r="BT84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Elliott et al. (2023)</t>
+          <t>Elliott et al., 2023</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -11671,7 +11781,11 @@
           <t>https://www.frontiersin.org/articles/10.3389/fmars.2023.1308689/full</t>
         </is>
       </c>
-      <c r="F85" t="inlineStr"/>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Central Atlantic|</t>
+        </is>
+      </c>
       <c r="G85" t="n">
         <v>1</v>
       </c>
@@ -11680,10 +11794,18 @@
           <t>Frontiers in Marine Science</t>
         </is>
       </c>
-      <c r="I85" t="inlineStr"/>
-      <c r="J85" t="inlineStr"/>
-      <c r="K85" t="inlineStr"/>
-      <c r="L85" t="inlineStr"/>
+      <c r="I85" t="n">
+        <v>13.6</v>
+      </c>
+      <c r="J85" t="n">
+        <v>13.6</v>
+      </c>
+      <c r="K85" t="n">
+        <v>-59.4</v>
+      </c>
+      <c r="L85" t="n">
+        <v>-59.4</v>
+      </c>
       <c r="M85" t="inlineStr">
         <is>
           <t>Fe, P,</t>
@@ -11759,11 +11881,12 @@
       <c r="BQ85" t="inlineStr"/>
       <c r="BR85" t="inlineStr"/>
       <c r="BS85" t="inlineStr"/>
+      <c r="BT85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Sakata et al. (2022)</t>
+          <t>Sakata et al., 2022</t>
         </is>
       </c>
       <c r="B86" t="n">
@@ -11784,7 +11907,11 @@
           <t>https://doi.org/10.5194/acp-22-9461-2022</t>
         </is>
       </c>
-      <c r="F86" t="inlineStr"/>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Central East Pacific| Central West Pacific| Australia Pacific| South Pacific|</t>
+        </is>
+      </c>
       <c r="G86" t="n">
         <v>1</v>
       </c>
@@ -11793,10 +11920,18 @@
           <t>Atmospheric Chemistry and Physics</t>
         </is>
       </c>
-      <c r="I86" t="inlineStr"/>
-      <c r="J86" t="inlineStr"/>
-      <c r="K86" t="inlineStr"/>
-      <c r="L86" t="inlineStr"/>
+      <c r="I86" t="n">
+        <v>-49.39</v>
+      </c>
+      <c r="J86" t="n">
+        <v>21.46</v>
+      </c>
+      <c r="K86" t="n">
+        <v>143.58</v>
+      </c>
+      <c r="L86" t="n">
+        <v>190</v>
+      </c>
       <c r="M86" t="inlineStr">
         <is>
           <t>Fe, N, Al,</t>
@@ -11876,11 +12011,12 @@
       <c r="BQ86" t="inlineStr"/>
       <c r="BR86" t="inlineStr"/>
       <c r="BS86" t="inlineStr"/>
+      <c r="BT86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Wang et al. (2022)</t>
+          <t>Wang Y. et al. (2022)</t>
         </is>
       </c>
       <c r="B87" t="n">
@@ -12015,6 +12151,7 @@
       <c r="BS87" t="n">
         <v>1</v>
       </c>
+      <c r="BT87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -12134,6 +12271,7 @@
       <c r="BQ88" t="inlineStr"/>
       <c r="BR88" t="inlineStr"/>
       <c r="BS88" t="inlineStr"/>
+      <c r="BT88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -12168,10 +12306,18 @@
           <t>NPJ Climate and Atmospheric Science</t>
         </is>
       </c>
-      <c r="I89" t="inlineStr"/>
-      <c r="J89" t="inlineStr"/>
-      <c r="K89" t="inlineStr"/>
-      <c r="L89" t="inlineStr"/>
+      <c r="I89" t="n">
+        <v>30.28</v>
+      </c>
+      <c r="J89" t="n">
+        <v>30.28</v>
+      </c>
+      <c r="K89" t="n">
+        <v>105.63</v>
+      </c>
+      <c r="L89" t="n">
+        <v>105.63</v>
+      </c>
       <c r="M89" t="inlineStr">
         <is>
           <t>Al,  Fe,  Mn,  Zn,  Cu,  Pb,  Cr,  As</t>
@@ -12263,6 +12409,7 @@
       <c r="BQ89" t="inlineStr"/>
       <c r="BR89" t="inlineStr"/>
       <c r="BS89" t="inlineStr"/>
+      <c r="BT89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -12288,7 +12435,11 @@
           <t>https://doi.org/10.5194/acp-23-10117-2023</t>
         </is>
       </c>
-      <c r="F90" t="inlineStr"/>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Bay of Bengal|</t>
+        </is>
+      </c>
       <c r="G90" t="n">
         <v>0</v>
       </c>
@@ -12297,10 +12448,18 @@
           <t>EGU Atmospheric Chemistry and Physics</t>
         </is>
       </c>
-      <c r="I90" t="inlineStr"/>
-      <c r="J90" t="inlineStr"/>
-      <c r="K90" t="inlineStr"/>
-      <c r="L90" t="inlineStr"/>
+      <c r="I90" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="J90" t="n">
+        <v>14.99</v>
+      </c>
+      <c r="K90" t="n">
+        <v>87.98</v>
+      </c>
+      <c r="L90" t="n">
+        <v>89.72</v>
+      </c>
       <c r="M90" t="inlineStr">
         <is>
           <t>Na,  Al,  K,  Ca,  Ti,  V,  Mn,  Fe,  Ni,  Zn</t>
@@ -12396,11 +12555,12 @@
       <c r="BQ90" t="inlineStr"/>
       <c r="BR90" t="inlineStr"/>
       <c r="BS90" t="inlineStr"/>
+      <c r="BT90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Kurisu et al. (2021)</t>
+          <t>Kurisu et al., 2021</t>
         </is>
       </c>
       <c r="B91" t="n">
@@ -12421,7 +12581,11 @@
           <t>https://doi.org/10.5194/acp-21-16027-2021</t>
         </is>
       </c>
-      <c r="F91" t="inlineStr"/>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Central West Pacific| Central Atlantic| Arctic Ocean|</t>
+        </is>
+      </c>
       <c r="G91" t="n">
         <v>1</v>
       </c>
@@ -12430,10 +12594,18 @@
           <t>Atmospheric Chemistry and Physics</t>
         </is>
       </c>
-      <c r="I91" t="inlineStr"/>
-      <c r="J91" t="inlineStr"/>
-      <c r="K91" t="inlineStr"/>
-      <c r="L91" t="inlineStr"/>
+      <c r="I91" t="n">
+        <v>5.63</v>
+      </c>
+      <c r="J91" t="n">
+        <v>62.06</v>
+      </c>
+      <c r="K91" t="n">
+        <v>141.1</v>
+      </c>
+      <c r="L91" t="n">
+        <v>289.585</v>
+      </c>
       <c r="M91" t="inlineStr">
         <is>
           <t>Fe,  Pb,  V,  Ti</t>
@@ -12513,6 +12685,7 @@
       <c r="BQ91" t="inlineStr"/>
       <c r="BR91" t="inlineStr"/>
       <c r="BS91" t="inlineStr"/>
+      <c r="BT91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -12640,11 +12813,12 @@
       <c r="BQ92" t="inlineStr"/>
       <c r="BR92" t="inlineStr"/>
       <c r="BS92" t="inlineStr"/>
+      <c r="BT92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Panda et al. (2022)</t>
+          <t>Panda et al., 2022</t>
         </is>
       </c>
       <c r="B93" t="n">
@@ -12665,7 +12839,11 @@
           <t>https://doi.org/10.1021/acsearthspacechem.2c00067</t>
         </is>
       </c>
-      <c r="F93" t="inlineStr"/>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Arabian Sea|</t>
+        </is>
+      </c>
       <c r="G93" t="n">
         <v>0</v>
       </c>
@@ -12674,10 +12852,18 @@
           <t>ACS Earth and Space Chemistry</t>
         </is>
       </c>
-      <c r="I93" t="inlineStr"/>
-      <c r="J93" t="inlineStr"/>
-      <c r="K93" t="inlineStr"/>
-      <c r="L93" t="inlineStr"/>
+      <c r="I93" t="n">
+        <v>11.17</v>
+      </c>
+      <c r="J93" t="n">
+        <v>20.71</v>
+      </c>
+      <c r="K93" t="n">
+        <v>66.02</v>
+      </c>
+      <c r="L93" t="n">
+        <v>75.23999999999999</v>
+      </c>
       <c r="M93" t="inlineStr">
         <is>
           <t>Fe,  Mn,  Cu</t>
@@ -12755,11 +12941,12 @@
       <c r="BQ93" t="inlineStr"/>
       <c r="BR93" t="inlineStr"/>
       <c r="BS93" t="inlineStr"/>
+      <c r="BT93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Marafante et al. (2024)</t>
+          <t>Marafante et al., 2024</t>
         </is>
       </c>
       <c r="B94" t="n">
@@ -12780,7 +12967,11 @@
           <t>https://www.ncbi.nlm.nih.gov/pubmed/38227013</t>
         </is>
       </c>
-      <c r="F94" t="inlineStr"/>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Arctic Ocean|</t>
+        </is>
+      </c>
       <c r="G94" t="n">
         <v>1</v>
       </c>
@@ -12789,10 +12980,18 @@
           <t>Analytical and Bioanalytical Chemistry</t>
         </is>
       </c>
-      <c r="I94" t="inlineStr"/>
-      <c r="J94" t="inlineStr"/>
-      <c r="K94" t="inlineStr"/>
-      <c r="L94" t="inlineStr"/>
+      <c r="I94" t="n">
+        <v>78.90000000000001</v>
+      </c>
+      <c r="J94" t="n">
+        <v>78.90000000000001</v>
+      </c>
+      <c r="K94" t="n">
+        <v>11.9</v>
+      </c>
+      <c r="L94" t="n">
+        <v>11.9</v>
+      </c>
       <c r="M94" t="inlineStr">
         <is>
           <t>Al,  Fe,  Cu,  Mn,  Zn,  Na,  K,  Mg,  Ca</t>
@@ -12886,6 +13085,7 @@
       <c r="BQ94" t="inlineStr"/>
       <c r="BR94" t="inlineStr"/>
       <c r="BS94" t="inlineStr"/>
+      <c r="BT94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -12911,7 +13111,11 @@
           <t>https://doi.org/10.1016/j.atmosenv.2021.118739</t>
         </is>
       </c>
-      <c r="F95" t="inlineStr"/>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Australia Pacific|</t>
+        </is>
+      </c>
       <c r="G95" t="n">
         <v>1</v>
       </c>
@@ -12920,10 +13124,18 @@
           <t>Atmospheric Environment</t>
         </is>
       </c>
-      <c r="I95" t="inlineStr"/>
-      <c r="J95" t="inlineStr"/>
-      <c r="K95" t="inlineStr"/>
-      <c r="L95" t="inlineStr"/>
+      <c r="I95" t="n">
+        <v>-33.796</v>
+      </c>
+      <c r="J95" t="n">
+        <v>-33.796</v>
+      </c>
+      <c r="K95" t="n">
+        <v>151.249</v>
+      </c>
+      <c r="L95" t="n">
+        <v>151.249</v>
+      </c>
       <c r="M95" t="inlineStr">
         <is>
           <t>Fe, N,</t>
@@ -13001,6 +13213,7 @@
       <c r="BQ95" t="inlineStr"/>
       <c r="BR95" t="inlineStr"/>
       <c r="BS95" t="inlineStr"/>
+      <c r="BT95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -13128,6 +13341,7 @@
       <c r="BQ96" t="inlineStr"/>
       <c r="BR96" t="inlineStr"/>
       <c r="BS96" t="inlineStr"/>
+      <c r="BT96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -13153,7 +13367,11 @@
           <t>https://www.ncbi.nlm.nih.gov/pubmed/35026325</t>
         </is>
       </c>
-      <c r="F97" t="inlineStr"/>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Central West Pacific|</t>
+        </is>
+      </c>
       <c r="G97" t="n">
         <v>1</v>
       </c>
@@ -13162,10 +13380,18 @@
           <t>Environmental Pollution</t>
         </is>
       </c>
-      <c r="I97" t="inlineStr"/>
-      <c r="J97" t="inlineStr"/>
-      <c r="K97" t="inlineStr"/>
-      <c r="L97" t="inlineStr"/>
+      <c r="I97" t="n">
+        <v>22.55</v>
+      </c>
+      <c r="J97" t="n">
+        <v>22.55</v>
+      </c>
+      <c r="K97" t="n">
+        <v>114.6</v>
+      </c>
+      <c r="L97" t="n">
+        <v>114.6</v>
+      </c>
       <c r="M97" t="inlineStr">
         <is>
           <t>N,</t>
@@ -13233,11 +13459,12 @@
       <c r="BQ97" t="inlineStr"/>
       <c r="BR97" t="inlineStr"/>
       <c r="BS97" t="inlineStr"/>
+      <c r="BT97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Zhang et al. (2024)</t>
+          <t>Zhang et al., 2024</t>
         </is>
       </c>
       <c r="B98" t="n">
@@ -13258,7 +13485,11 @@
           <t>https://www.ncbi.nlm.nih.gov/pubmed/38092217</t>
         </is>
       </c>
-      <c r="F98" t="inlineStr"/>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Central West Pacific| Western North Pacific|</t>
+        </is>
+      </c>
       <c r="G98" t="n">
         <v>1</v>
       </c>
@@ -13267,13 +13498,21 @@
           <t>Science of Total Environment</t>
         </is>
       </c>
-      <c r="I98" t="inlineStr"/>
-      <c r="J98" t="inlineStr"/>
-      <c r="K98" t="inlineStr"/>
-      <c r="L98" t="inlineStr"/>
+      <c r="I98" t="n">
+        <v>27</v>
+      </c>
+      <c r="J98" t="n">
+        <v>34</v>
+      </c>
+      <c r="K98" t="n">
+        <v>121</v>
+      </c>
+      <c r="L98" t="n">
+        <v>149</v>
+      </c>
       <c r="M98" t="inlineStr">
         <is>
-          <t xml:space="preserve">K,  Fe,  Ca,  Zn,  Mn,  Ba,  Pb,  V,  Ni,  As,  Se,  Cd, </t>
+          <t>K,  Fe,  Ca,  Zn,  Mn,  Ba,  Pb,  V,  Ni,  As,  Se,  Cd</t>
         </is>
       </c>
       <c r="N98" t="inlineStr"/>
@@ -13366,6 +13605,7 @@
       <c r="BQ98" t="inlineStr"/>
       <c r="BR98" t="inlineStr"/>
       <c r="BS98" t="inlineStr"/>
+      <c r="BT98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -13489,11 +13729,12 @@
       <c r="BQ99" t="inlineStr"/>
       <c r="BR99" t="inlineStr"/>
       <c r="BS99" t="inlineStr"/>
+      <c r="BT99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>López-García et al. (2021)</t>
+          <t>Lopez-Garcia et al., 2021</t>
         </is>
       </c>
       <c r="B100" t="n">
@@ -13514,7 +13755,11 @@
           <t>https://linkinghub.elsevier.com/retrieve/pii/S1352231020308220</t>
         </is>
       </c>
-      <c r="F100" t="inlineStr"/>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Central Atlantic|</t>
+        </is>
+      </c>
       <c r="G100" t="n">
         <v>1</v>
       </c>
@@ -13523,10 +13768,18 @@
           <t>Atmospheric Environment</t>
         </is>
       </c>
-      <c r="I100" t="inlineStr"/>
-      <c r="J100" t="inlineStr"/>
-      <c r="K100" t="inlineStr"/>
-      <c r="L100" t="inlineStr"/>
+      <c r="I100" t="n">
+        <v>28.1</v>
+      </c>
+      <c r="J100" t="n">
+        <v>28.1</v>
+      </c>
+      <c r="K100" t="n">
+        <v>15.4</v>
+      </c>
+      <c r="L100" t="n">
+        <v>15.4</v>
+      </c>
       <c r="M100" t="inlineStr">
         <is>
           <t>Fe,  N,  P</t>
@@ -13606,11 +13859,12 @@
       <c r="BQ100" t="inlineStr"/>
       <c r="BR100" t="inlineStr"/>
       <c r="BS100" t="inlineStr"/>
+      <c r="BT100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Wang et al. (2022)</t>
+          <t>Wang X. et al. (2022)</t>
         </is>
       </c>
       <c r="B101" t="n">
@@ -13631,7 +13885,11 @@
           <t>https://www.ncbi.nlm.nih.gov/pubmed/36195196</t>
         </is>
       </c>
-      <c r="F101" t="inlineStr"/>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Central West Pacific| Western North Pacific|</t>
+        </is>
+      </c>
       <c r="G101" t="n">
         <v>1</v>
       </c>
@@ -13640,10 +13898,18 @@
           <t>Environmental Pollution</t>
         </is>
       </c>
-      <c r="I101" t="inlineStr"/>
-      <c r="J101" t="inlineStr"/>
-      <c r="K101" t="inlineStr"/>
-      <c r="L101" t="inlineStr"/>
+      <c r="I101" t="n">
+        <v>23.12</v>
+      </c>
+      <c r="J101" t="n">
+        <v>45.74</v>
+      </c>
+      <c r="K101" t="n">
+        <v>104.06</v>
+      </c>
+      <c r="L101" t="n">
+        <v>126.73</v>
+      </c>
       <c r="M101" t="inlineStr">
         <is>
           <t>Fe, N,</t>
@@ -13721,6 +13987,7 @@
       <c r="BQ101" t="inlineStr"/>
       <c r="BR101" t="inlineStr"/>
       <c r="BS101" t="inlineStr"/>
+      <c r="BT101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -13842,6 +14109,7 @@
       <c r="BQ102" t="inlineStr"/>
       <c r="BR102" t="inlineStr"/>
       <c r="BS102" t="inlineStr"/>
+      <c r="BT102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -13867,7 +14135,11 @@
           <t>https://www.mdpi.com/2073-4433/14/1/102</t>
         </is>
       </c>
-      <c r="F103" t="inlineStr"/>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Central East Pacific| Central Atlantic|</t>
+        </is>
+      </c>
       <c r="G103" t="n">
         <v>1</v>
       </c>
@@ -13876,13 +14148,21 @@
           <t>Atmosphere</t>
         </is>
       </c>
-      <c r="I103" t="inlineStr"/>
-      <c r="J103" t="inlineStr"/>
-      <c r="K103" t="inlineStr"/>
-      <c r="L103" t="inlineStr"/>
+      <c r="I103" t="n">
+        <v>26.497</v>
+      </c>
+      <c r="J103" t="n">
+        <v>26.497</v>
+      </c>
+      <c r="K103" t="n">
+        <v>-81.751</v>
+      </c>
+      <c r="L103" t="n">
+        <v>-81.751</v>
+      </c>
       <c r="M103" t="inlineStr">
         <is>
-          <t>Al,  Si,  Fe,  K,  Ca,  Mg,  P,  N</t>
+          <t>Al,  Si,  Fe,  K,  Ca,  Mg,  P,  N,  B,  Cu,  Cr</t>
         </is>
       </c>
       <c r="N103" t="inlineStr"/>
@@ -13909,7 +14189,9 @@
       <c r="U103" t="n">
         <v>1</v>
       </c>
-      <c r="V103" t="inlineStr"/>
+      <c r="V103" t="n">
+        <v>1</v>
+      </c>
       <c r="W103" t="inlineStr"/>
       <c r="X103" t="inlineStr"/>
       <c r="Y103" t="inlineStr"/>
@@ -13932,7 +14214,9 @@
       <c r="AH103" t="inlineStr"/>
       <c r="AI103" t="inlineStr"/>
       <c r="AJ103" t="inlineStr"/>
-      <c r="AK103" t="inlineStr"/>
+      <c r="AK103" t="n">
+        <v>1</v>
+      </c>
       <c r="AL103" t="inlineStr"/>
       <c r="AM103" t="inlineStr"/>
       <c r="AN103" t="inlineStr"/>
@@ -13967,11 +14251,14 @@
       <c r="BQ103" t="inlineStr"/>
       <c r="BR103" t="inlineStr"/>
       <c r="BS103" t="inlineStr"/>
+      <c r="BT103" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Desboeufs et al. (2024)</t>
+          <t>Desboeufs et al., 2024</t>
         </is>
       </c>
       <c r="B104" t="n">
@@ -13992,7 +14279,11 @@
           <t>https://acp.copernicus.org/articles/24/1525/2024/</t>
         </is>
       </c>
-      <c r="F104" t="inlineStr"/>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> South Atlantic|</t>
+        </is>
+      </c>
       <c r="G104" t="n">
         <v>1</v>
       </c>
@@ -14001,10 +14292,18 @@
           <t>Atmospheric Chemistry and Physics</t>
         </is>
       </c>
-      <c r="I104" t="inlineStr"/>
-      <c r="J104" t="inlineStr"/>
-      <c r="K104" t="inlineStr"/>
-      <c r="L104" t="inlineStr"/>
+      <c r="I104" t="n">
+        <v>-22.09</v>
+      </c>
+      <c r="J104" t="n">
+        <v>-22.09</v>
+      </c>
+      <c r="K104" t="n">
+        <v>14.26</v>
+      </c>
+      <c r="L104" t="n">
+        <v>14.26</v>
+      </c>
       <c r="M104" t="inlineStr">
         <is>
           <t>Fe,  Al,  Si,  N</t>
@@ -14086,11 +14385,12 @@
       <c r="BQ104" t="inlineStr"/>
       <c r="BR104" t="inlineStr"/>
       <c r="BS104" t="inlineStr"/>
+      <c r="BT104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Rodríguez et al. (2021)</t>
+          <t>Rodriguez et al., 2021</t>
         </is>
       </c>
       <c r="B105" t="n">
@@ -14111,7 +14411,11 @@
           <t>https://doi.org/10.1016/j.atmosenv.2020.118092</t>
         </is>
       </c>
-      <c r="F105" t="inlineStr"/>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Central East Pacific| Central Atlantic|</t>
+        </is>
+      </c>
       <c r="G105" t="n">
         <v>1</v>
       </c>
@@ -14120,10 +14424,18 @@
           <t>Atmospheric Environment</t>
         </is>
       </c>
-      <c r="I105" t="inlineStr"/>
-      <c r="J105" t="inlineStr"/>
-      <c r="K105" t="inlineStr"/>
-      <c r="L105" t="inlineStr"/>
+      <c r="I105" t="n">
+        <v>13.165</v>
+      </c>
+      <c r="J105" t="n">
+        <v>25.732</v>
+      </c>
+      <c r="K105" t="n">
+        <v>279.84</v>
+      </c>
+      <c r="L105" t="n">
+        <v>343.5</v>
+      </c>
       <c r="M105" t="inlineStr">
         <is>
           <t>Fe,  Al,  N</t>
@@ -14203,11 +14515,12 @@
       <c r="BQ105" t="inlineStr"/>
       <c r="BR105" t="inlineStr"/>
       <c r="BS105" t="inlineStr"/>
+      <c r="BT105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Seo et al. (2023)</t>
+          <t>Seo &amp; Kim, 2023</t>
         </is>
       </c>
       <c r="B106" t="n">
@@ -14228,7 +14541,11 @@
           <t>https://www.ncbi.nlm.nih.gov/pubmed/37435964</t>
         </is>
       </c>
-      <c r="F106" t="inlineStr"/>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Western North Pacific|</t>
+        </is>
+      </c>
       <c r="G106" t="n">
         <v>0</v>
       </c>
@@ -14237,10 +14554,18 @@
           <t>Environmental Science and Technology</t>
         </is>
       </c>
-      <c r="I106" t="inlineStr"/>
-      <c r="J106" t="inlineStr"/>
-      <c r="K106" t="inlineStr"/>
-      <c r="L106" t="inlineStr"/>
+      <c r="I106" t="n">
+        <v>37.08</v>
+      </c>
+      <c r="J106" t="n">
+        <v>37.08</v>
+      </c>
+      <c r="K106" t="n">
+        <v>129.41</v>
+      </c>
+      <c r="L106" t="n">
+        <v>129.41</v>
+      </c>
       <c r="M106" t="inlineStr">
         <is>
           <t>Na,  Al,  K,  Fe,  V,  Ni,  and Pb</t>
@@ -14326,11 +14651,12 @@
       <c r="BQ106" t="inlineStr"/>
       <c r="BR106" t="inlineStr"/>
       <c r="BS106" t="inlineStr"/>
+      <c r="BT106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Wu et al. (2023)</t>
+          <t>Wu, Hsieh, and Ho et al., 2023</t>
         </is>
       </c>
       <c r="B107" t="n">
@@ -14351,7 +14677,11 @@
           <t>https://doi.org/10.1016/j.marchem.2023.104277</t>
         </is>
       </c>
-      <c r="F107" t="inlineStr"/>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Central West Pacific|</t>
+        </is>
+      </c>
       <c r="G107" t="n">
         <v>1</v>
       </c>
@@ -14360,10 +14690,18 @@
           <t>Marine Chemistry</t>
         </is>
       </c>
-      <c r="I107" t="inlineStr"/>
-      <c r="J107" t="inlineStr"/>
-      <c r="K107" t="inlineStr"/>
-      <c r="L107" t="inlineStr"/>
+      <c r="I107" t="n">
+        <v>26.17</v>
+      </c>
+      <c r="J107" t="n">
+        <v>26.17</v>
+      </c>
+      <c r="K107" t="n">
+        <v>119.92</v>
+      </c>
+      <c r="L107" t="n">
+        <v>119.92</v>
+      </c>
       <c r="M107" t="inlineStr">
         <is>
           <t>Fe,  Pb,  Al,  Cd,  Zn,  Mn,  Co,  Ni</t>
@@ -14451,11 +14789,12 @@
       <c r="BQ107" t="inlineStr"/>
       <c r="BR107" t="inlineStr"/>
       <c r="BS107" t="inlineStr"/>
+      <c r="BT107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Winton et al. (2022)</t>
+          <t>Winton et al., 2022</t>
         </is>
       </c>
       <c r="B108" t="n">
@@ -14476,7 +14815,11 @@
           <t>https://doi.org/10.1029/2022JD036586</t>
         </is>
       </c>
-      <c r="F108" t="inlineStr"/>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Arctic Ocean|</t>
+        </is>
+      </c>
       <c r="G108" t="n">
         <v>1</v>
       </c>
@@ -14485,10 +14828,18 @@
           <t>JGR Atmospheres</t>
         </is>
       </c>
-      <c r="I108" t="inlineStr"/>
-      <c r="J108" t="inlineStr"/>
-      <c r="K108" t="inlineStr"/>
-      <c r="L108" t="inlineStr"/>
+      <c r="I108" t="n">
+        <v>71.2</v>
+      </c>
+      <c r="J108" t="n">
+        <v>71.2</v>
+      </c>
+      <c r="K108" t="n">
+        <v>110.5</v>
+      </c>
+      <c r="L108" t="n">
+        <v>110.5</v>
+      </c>
       <c r="M108" t="inlineStr">
         <is>
           <t>Na,  Ti,  Al,  Fe,  Pb</t>
@@ -14570,11 +14921,12 @@
       <c r="BQ108" t="inlineStr"/>
       <c r="BR108" t="inlineStr"/>
       <c r="BS108" t="inlineStr"/>
+      <c r="BT108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Srinivas et al. (2012)</t>
+          <t xml:space="preserve">Srinivas, Sarin, and Kumar 2012 </t>
         </is>
       </c>
       <c r="B109" t="n">
@@ -14595,7 +14947,11 @@
           <t>https://doi.org/10.1007/s10533-011-9680-1</t>
         </is>
       </c>
-      <c r="F109" t="inlineStr"/>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Bay of Bengal|</t>
+        </is>
+      </c>
       <c r="G109" t="n">
         <v>1</v>
       </c>
@@ -14604,10 +14960,18 @@
           <t>Biogeochemistry</t>
         </is>
       </c>
-      <c r="I109" t="inlineStr"/>
-      <c r="J109" t="inlineStr"/>
-      <c r="K109" t="inlineStr"/>
-      <c r="L109" t="inlineStr"/>
+      <c r="I109" t="n">
+        <v>13.13</v>
+      </c>
+      <c r="J109" t="n">
+        <v>13.13</v>
+      </c>
+      <c r="K109" t="n">
+        <v>87.38</v>
+      </c>
+      <c r="L109" t="n">
+        <v>87.38</v>
+      </c>
       <c r="M109" t="inlineStr">
         <is>
           <t>Al,  Ca,  Cd,  Mg,  Pb</t>
@@ -14695,6 +15059,7 @@
       <c r="BQ109" t="inlineStr"/>
       <c r="BR109" t="inlineStr"/>
       <c r="BS109" t="inlineStr"/>
+      <c r="BT109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -14756,8 +15121,10 @@
       <c r="O110" t="n">
         <v>1</v>
       </c>
-      <c r="P110" t="b">
-        <v>1</v>
+      <c r="P110" t="inlineStr">
+        <is>
+          <t>Soluble</t>
+        </is>
       </c>
       <c r="Q110" t="inlineStr">
         <is>
@@ -14822,6 +15189,7 @@
       <c r="BQ110" t="inlineStr"/>
       <c r="BR110" t="inlineStr"/>
       <c r="BS110" t="inlineStr"/>
+      <c r="BT110" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>